<commit_message>
add delete classroom when import file
</commit_message>
<xml_diff>
--- a/importfile.xlsx
+++ b/importfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\project-novriani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCDB557-3D15-4BD1-ADE6-0B1EDC94029F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B2A6B-FF2A-491C-8E98-4B2020E237A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nama</t>
   </si>
@@ -57,7 +57,16 @@
     <t>Nature Rep</t>
   </si>
   <si>
-    <t>1c</t>
+    <t>2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminator </t>
+  </si>
+  <si>
+    <t>Orico</t>
+  </si>
+  <si>
+    <t>1e</t>
   </si>
 </sst>
 </file>
@@ -377,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +429,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -446,7 +455,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -464,6 +473,58 @@
         <v>89</v>
       </c>
       <c r="H3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
         <v>100</v>
       </c>
     </row>

</xml_diff>